<commit_message>
testcases 1 and 2 merged
</commit_message>
<xml_diff>
--- a/testData/Output.xlsx
+++ b/testData/Output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2408395_cognizant_com/Documents/Desktop/Final_Project/HackathonProject/testData/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Book Shelve Name</t>
   </si>
@@ -66,6 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,8 +454,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0"/>
+    <col min="2" max="2" customWidth="true" width="13.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -466,26 +467,26 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed method names and modified testcases
</commit_message>
<xml_diff>
--- a/testData/Output.xlsx
+++ b/testData/Output.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2408395_cognizant_com/Documents/Desktop/Final_Project/HackathonProject/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{582A54B8-0ED4-48C6-BA06-CA5E26CDED99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D43724F-5B84-4A81-B870-5CC87FE429B9}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{582A54B8-0ED4-48C6-BA06-CA5E26CDED99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF80A137-BC30-4786-9C05-4EE12ACA7332}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{D56685F8-8774-40F8-9DB8-9BBB5FDDCA05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>Book Shelve Name</t>
   </si>
@@ -59,7 +61,49 @@
     <t>Helios Amante Mango Wood Book Shelf - Brown</t>
   </si>
   <si>
-    <t>11,373</t>
+    <t>8,999</t>
+  </si>
+  <si>
+    <t>Home Accessories Items</t>
+  </si>
+  <si>
+    <t>Login Error Message</t>
+  </si>
+  <si>
+    <t>Email must be a valid email address.</t>
+  </si>
+  <si>
+    <t>Candle Holders And Lanterns</t>
+  </si>
+  <si>
+    <t>Clocks</t>
+  </si>
+  <si>
+    <t>Desk Accessories</t>
+  </si>
+  <si>
+    <t>Figurines</t>
+  </si>
+  <si>
+    <t>Gift Accessories</t>
+  </si>
+  <si>
+    <t>Lamps</t>
+  </si>
+  <si>
+    <t>Mirrors</t>
+  </si>
+  <si>
+    <t>Ornaments</t>
+  </si>
+  <si>
+    <t>Potpouri Bowl and Platter</t>
+  </si>
+  <si>
+    <t>Midori Bamboo 5-Tier Book Shelf - Light Brown</t>
+  </si>
+  <si>
+    <t>4,997</t>
   </si>
 </sst>
 </file>
@@ -129,6 +173,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -468,26 +516,122 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEC3163-1637-4D4E-8EC8-12BA0E28AFE8}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="41.7265625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D45B881-FFE0-45ED-AFF3-AA283A3ABC4E}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="43.54296875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>